<commit_message>
working on adding thermistors but encountered too many hierarchicaly copies bug
</commit_message>
<xml_diff>
--- a/motor_drive_REV_1/notes/BOM.xlsx
+++ b/motor_drive_REV_1/notes/BOM.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18312\Desktop\KiCad\motor_drive\motor_drive_REV_1\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF21462-0579-435C-8E68-4530E6692399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B36D6C-B870-4C4A-B96D-D41F97C3935B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="300" windowWidth="14745" windowHeight="15300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="135" yWindow="120" windowWidth="12315" windowHeight="15300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="rooms" sheetId="4" r:id="rId1"/>
+    <sheet name="Specs" sheetId="6" r:id="rId1"/>
     <sheet name="full list" sheetId="1" r:id="rId2"/>
     <sheet name="top_pick" sheetId="2" r:id="rId3"/>
-    <sheet name="F28027 pin assignment" sheetId="3" r:id="rId4"/>
+    <sheet name="rooms" sheetId="4" r:id="rId4"/>
+    <sheet name="F28027 pin assignment" sheetId="3" r:id="rId5"/>
+    <sheet name="RC calcs" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="252">
   <si>
     <t>Category</t>
   </si>
@@ -225,9 +227,6 @@
     <t>U9</t>
   </si>
   <si>
-    <t>C16</t>
-  </si>
-  <si>
     <t>C23</t>
   </si>
   <si>
@@ -634,6 +633,165 @@
   </si>
   <si>
     <t>ADC_B7</t>
+  </si>
+  <si>
+    <t>room_TMS</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>L2</t>
+  </si>
+  <si>
+    <t>C31</t>
+  </si>
+  <si>
+    <t>C32</t>
+  </si>
+  <si>
+    <t>R31</t>
+  </si>
+  <si>
+    <t>R33</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>R38</t>
+  </si>
+  <si>
+    <t>R40</t>
+  </si>
+  <si>
+    <t>R42</t>
+  </si>
+  <si>
+    <t>R44</t>
+  </si>
+  <si>
+    <t>R46</t>
+  </si>
+  <si>
+    <t>R48</t>
+  </si>
+  <si>
+    <t>R50</t>
+  </si>
+  <si>
+    <t>R35</t>
+  </si>
+  <si>
+    <t>R37</t>
+  </si>
+  <si>
+    <t>R39</t>
+  </si>
+  <si>
+    <t>R41</t>
+  </si>
+  <si>
+    <t>R43</t>
+  </si>
+  <si>
+    <t>R45</t>
+  </si>
+  <si>
+    <t>R47</t>
+  </si>
+  <si>
+    <t>R49</t>
+  </si>
+  <si>
+    <t>VDD1</t>
+  </si>
+  <si>
+    <t>C24</t>
+  </si>
+  <si>
+    <t>C26</t>
+  </si>
+  <si>
+    <t>VDD2</t>
+  </si>
+  <si>
+    <t>C25</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>Q6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>R9</t>
+  </si>
+  <si>
+    <t>room_FAN7888</t>
+  </si>
+  <si>
+    <t>C21</t>
+  </si>
+  <si>
+    <t>C22</t>
+  </si>
+  <si>
+    <t>D1</t>
+  </si>
+  <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>freq</t>
+  </si>
+  <si>
+    <t>C34</t>
+  </si>
+  <si>
+    <t>C35</t>
+  </si>
+  <si>
+    <t>param</t>
+  </si>
+  <si>
+    <t>specification</t>
+  </si>
+  <si>
+    <t>DC voltage</t>
+  </si>
+  <si>
+    <t>40v nom, 60v max</t>
+  </si>
+  <si>
+    <t>DC current</t>
+  </si>
+  <si>
+    <t>2A continuous, 5A peak</t>
+  </si>
+  <si>
+    <t>3A continuous, 8A peak</t>
+  </si>
+  <si>
+    <t>100 watts continuous, 250 watts peak</t>
+  </si>
+  <si>
+    <t>phase current</t>
   </si>
 </sst>
 </file>
@@ -959,7 +1117,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1084,6 +1242,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1363,143 +1533,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841E9C4-CA72-470B-B30B-420123CAEE39}">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D8B458A-86D8-40B9-BD4F-710A5D54850A}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>243</v>
       </c>
       <c r="B1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-      <c r="D2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>56</v>
+        <v>247</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" t="s">
-        <v>74</v>
-      </c>
-      <c r="C6" t="s">
-        <v>75</v>
-      </c>
-      <c r="D6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>77</v>
-      </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E7" t="s">
-        <v>83</v>
-      </c>
-      <c r="F7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>79</v>
+        <v>250</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1508,7 +1595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
@@ -2030,10 +2117,357 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4841E9C4-CA72-470B-B30B-420123CAEE39}">
+  <dimension ref="A1:K17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="44" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>241</v>
+      </c>
+      <c r="D2" s="46" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="48" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" s="49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D6" s="49" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="48" t="s">
+        <v>84</v>
+      </c>
+      <c r="C8" s="48" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="48" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="51" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="51" t="s">
+        <v>228</v>
+      </c>
+      <c r="D9" s="51" t="s">
+        <v>229</v>
+      </c>
+      <c r="E9" s="51" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="44" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="45"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="45"/>
+      <c r="K10" s="46"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="B11" s="48" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" s="48" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" s="48" t="s">
+        <v>224</v>
+      </c>
+      <c r="E11" s="48"/>
+      <c r="F11" s="48"/>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="48"/>
+      <c r="J11" s="48"/>
+      <c r="K11" s="49"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12" s="48" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" s="48" t="s">
+        <v>202</v>
+      </c>
+      <c r="D12" s="48" t="s">
+        <v>203</v>
+      </c>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="49"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>204</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>205</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>206</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>209</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>210</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>211</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>212</v>
+      </c>
+      <c r="K13" s="49" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="B14" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="E14" s="48" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" s="48" t="s">
+        <v>218</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>219</v>
+      </c>
+      <c r="H14" s="48" t="s">
+        <v>220</v>
+      </c>
+      <c r="I14" s="48" t="s">
+        <v>221</v>
+      </c>
+      <c r="J14" s="48"/>
+      <c r="K14" s="49"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="47" t="s">
+        <v>222</v>
+      </c>
+      <c r="B15" s="48" t="s">
+        <v>233</v>
+      </c>
+      <c r="C15" s="48" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="49"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="50" t="s">
+        <v>225</v>
+      </c>
+      <c r="B16" s="51" t="s">
+        <v>234</v>
+      </c>
+      <c r="C16" s="51" t="s">
+        <v>223</v>
+      </c>
+      <c r="D16" s="51"/>
+      <c r="E16" s="51"/>
+      <c r="F16" s="51"/>
+      <c r="G16" s="51"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
+      <c r="K16" s="52"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="53" t="s">
+        <v>232</v>
+      </c>
+      <c r="B17" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="C17" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>233</v>
+      </c>
+      <c r="E17" s="54" t="s">
+        <v>234</v>
+      </c>
+      <c r="F17" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="G17" s="54" t="s">
+        <v>235</v>
+      </c>
+      <c r="H17" s="54" t="s">
+        <v>236</v>
+      </c>
+      <c r="I17" s="54" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3082D45B-D41F-4E76-8A53-86D42592906D}">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
@@ -2049,22 +2483,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B1" s="38" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="38" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="38" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="38" t="s">
-        <v>116</v>
-      </c>
       <c r="E1" s="38" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F1" s="39" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2072,16 +2506,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C2" s="33" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D2" s="33" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E2" s="33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F2" s="40"/>
     </row>
@@ -2090,16 +2524,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C3" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D3" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F3" s="41"/>
     </row>
@@ -2108,19 +2542,19 @@
         <v>3</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="31" t="s">
         <v>12</v>
       </c>
       <c r="D4" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F4" s="41" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -2128,19 +2562,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="D5" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="C5" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>104</v>
-      </c>
       <c r="F5" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -2148,19 +2582,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F6" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2168,19 +2602,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F7" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2188,19 +2622,19 @@
         <v>7</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F8" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -2208,19 +2642,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E9" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F9" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -2228,19 +2662,19 @@
         <v>9</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E10" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -2248,19 +2682,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E11" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F11" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -2268,19 +2702,19 @@
         <v>11</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C12" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E12" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F12" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -2288,19 +2722,19 @@
         <v>12</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="36" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E13" s="36" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F13" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -2308,19 +2742,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F14" s="40" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2328,19 +2762,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E15" s="31" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F15" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -2348,19 +2782,19 @@
         <v>15</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C16" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E16" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F16" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -2368,19 +2802,19 @@
         <v>16</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E17" s="31" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -2388,19 +2822,19 @@
         <v>17</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E18" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F18" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -2408,19 +2842,19 @@
         <v>18</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E19" s="31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F19" s="41" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -2428,16 +2862,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C20" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E20" s="31" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F20" s="41"/>
     </row>
@@ -2446,16 +2880,16 @@
         <v>20</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E21" s="31" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F21" s="41"/>
     </row>
@@ -2464,16 +2898,16 @@
         <v>21</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C22" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E22" s="31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F22" s="41"/>
     </row>
@@ -2482,16 +2916,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E23" s="31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F23" s="41"/>
     </row>
@@ -2500,16 +2934,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E24" s="31" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F24" s="41"/>
     </row>
@@ -2518,16 +2952,16 @@
         <v>24</v>
       </c>
       <c r="B25" s="36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C25" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D25" s="36" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="E25" s="36" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F25" s="42"/>
     </row>
@@ -2536,16 +2970,16 @@
         <v>25</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F26" s="40"/>
     </row>
@@ -2554,16 +2988,16 @@
         <v>26</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E27" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F27" s="41"/>
     </row>
@@ -2572,16 +3006,16 @@
         <v>27</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28" s="31" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F28" s="41"/>
     </row>
@@ -2590,16 +3024,16 @@
         <v>28</v>
       </c>
       <c r="B29" s="31" t="s">
+        <v>177</v>
+      </c>
+      <c r="C29" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="D29" s="31" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="31" t="s">
         <v>178</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>156</v>
-      </c>
-      <c r="D29" s="31" t="s">
-        <v>154</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>179</v>
       </c>
       <c r="F29" s="41"/>
     </row>
@@ -2608,16 +3042,16 @@
         <v>29</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C30" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F30" s="41"/>
     </row>
@@ -2626,19 +3060,19 @@
         <v>30</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C31" s="31" t="s">
         <v>12</v>
       </c>
       <c r="D31" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E31" s="31" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F31" s="41" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -2646,16 +3080,16 @@
         <v>31</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C32" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D32" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F32" s="41"/>
     </row>
@@ -2664,19 +3098,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F33" s="41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2684,16 +3118,16 @@
         <v>33</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C34" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D34" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F34" s="41"/>
     </row>
@@ -2702,19 +3136,19 @@
         <v>34</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C35" s="31" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E35" s="31" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F35" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2722,19 +3156,19 @@
         <v>35</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C36" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D36" s="31" t="s">
+        <v>158</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="F36" s="41" t="s">
         <v>159</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="F36" s="41" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2742,16 +3176,16 @@
         <v>36</v>
       </c>
       <c r="B37" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D37" s="36" t="s">
+        <v>160</v>
+      </c>
+      <c r="E37" s="36" t="s">
         <v>161</v>
-      </c>
-      <c r="E37" s="36" t="s">
-        <v>162</v>
       </c>
       <c r="F37" s="42"/>
     </row>
@@ -2760,16 +3194,16 @@
         <v>37</v>
       </c>
       <c r="B38" s="33" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C38" s="33" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D38" s="33" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E38" s="33" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F38" s="40"/>
     </row>
@@ -2778,16 +3212,16 @@
         <v>38</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D39" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E39" s="31" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="F39" s="41"/>
     </row>
@@ -2796,16 +3230,16 @@
         <v>39</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C40" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E40" s="31" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F40" s="41"/>
     </row>
@@ -2814,16 +3248,16 @@
         <v>40</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D41" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E41" s="31" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F41" s="41"/>
     </row>
@@ -2832,16 +3266,16 @@
         <v>41</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C42" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D42" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F42" s="41"/>
     </row>
@@ -2850,16 +3284,16 @@
         <v>42</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E43" s="31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F43" s="41"/>
     </row>
@@ -2868,19 +3302,19 @@
         <v>43</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C44" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D44" s="31" t="s">
         <v>12</v>
       </c>
       <c r="E44" s="31" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F44" s="41" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -2888,16 +3322,16 @@
         <v>44</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D45" s="31" t="s">
         <v>12</v>
       </c>
       <c r="E45" s="31" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F45" s="41"/>
     </row>
@@ -2906,19 +3340,19 @@
         <v>45</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C46" s="31" t="s">
         <v>12</v>
       </c>
       <c r="D46" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E46" s="31" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F46" s="41" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -2926,19 +3360,19 @@
         <v>46</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C47" s="31" t="s">
         <v>12</v>
       </c>
       <c r="D47" s="31" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E47" s="31" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F47" s="41" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -2946,16 +3380,16 @@
         <v>47</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C48" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E48" s="31" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F48" s="41"/>
     </row>
@@ -2964,18 +3398,56 @@
         <v>48</v>
       </c>
       <c r="B49" s="36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D49" s="36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E49" s="36" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F49" s="42"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1926ADC-9EED-4EAE-B3E8-806E5016EB8A}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C1" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2E-3</v>
+      </c>
+      <c r="B2" s="55">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="C2" s="55">
+        <f>(1/6.28)*(1/(A2*B2))</f>
+        <v>796178343.94904459</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
second try at layout
</commit_message>
<xml_diff>
--- a/motor_drive_REV_1/notes/BOM.xlsx
+++ b/motor_drive_REV_1/notes/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\18312\Desktop\KiCad\motor_drive\motor_drive_REV_1\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C79D28-4C5B-4570-85F7-2CE680D37A20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D215517F-F4FD-4AD2-955E-1301F6FFFB5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="135" yWindow="120" windowWidth="18435" windowHeight="15300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="1020" windowWidth="24030" windowHeight="15180" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Specs" sheetId="6" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="283">
   <si>
     <t>Category</t>
   </si>
@@ -879,6 +879,12 @@
   </si>
   <si>
     <t>GRJ21BC72A105KE11L</t>
+  </si>
+  <si>
+    <t>buck</t>
+  </si>
+  <si>
+    <t>TPSM265R1</t>
   </si>
 </sst>
 </file>
@@ -1980,7 +1986,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2369,8 +2375,12 @@
       <c r="H27" s="58"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="57"/>
-      <c r="B28" s="44"/>
+      <c r="A28" s="57" t="s">
+        <v>281</v>
+      </c>
+      <c r="B28" s="44" t="s">
+        <v>282</v>
+      </c>
       <c r="C28" s="44"/>
       <c r="D28" s="44"/>
       <c r="E28" s="44"/>

</xml_diff>